<commit_message>
mybatis generator usage modified
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>◆Spring Boot 模板</t>
   </si>
@@ -126,17 +126,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>配置文件和属性文件修改</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>src\main\resources</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>application.properties</t>
-  </si>
-  <si>
     <r>
       <t>打开pom.xml、将所有的template改</t>
     </r>
@@ -283,38 +272,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <r>
-      <t>数据</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>库连</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>接配置修改</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&lt;工程package名&gt;</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>主程序改名：TemplateApplicationTests.java -&gt; &lt;工程名&gt;ApplicationTests.java</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -399,78 +356,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t xml:space="preserve">&lt;com.gq.template&gt; </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>git clone https://github.com/ganquanjp/template.git</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>spring.datasource.schema=&lt;schema&gt;</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mybatis-generator-config.xml</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>postgresql-42.3.3.jar</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>以下三个文件用于开</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>发时生成所有数据库表的对象</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>产环</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>境不需要</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mybatis-generator.properties</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>mybatis已配置</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -483,6 +372,194 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>⑤</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">修改git </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>远</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>程url</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>查</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>看git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>远</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>程url</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>git remote -v</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>⑥</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>git push -u origin master</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>git remote set-url origin https://github.com/ganquanjp/&lt;工程名&gt;.git</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>在github上新建一个repository，与jenkins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>连</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>携的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>话</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>要</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>设</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>置Webhooks</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>将生成的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>象copy到工程中</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <r>
       <t>用mybatis-generator工具生</t>
     </r>
@@ -495,169 +572,76 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>产所有数据表的对象</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>⑤</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">修改git </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>远</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>程url</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>查</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>看git</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>远</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>程url</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>git remote -v</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>⑥</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>git push -u origin master</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>git remote set-url origin https://github.com/ganquanjp/&lt;工程名&gt;.git</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>在github上新建一个repository，与jenkins</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>连</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>携的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>话</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>要</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>设</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>置Webhooks</t>
-    </r>
+      <t>产</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>所有数据表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>象</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>参照mybatis-generator目</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>录</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>下的README.txt</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>src\main\resources\application.properties</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>主配置文件修改</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -717,11 +701,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1056,7 +1037,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -1064,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
@@ -1081,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I56"/>
+  <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1098,15 +1079,15 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -1117,7 +1098,7 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
@@ -1129,26 +1110,26 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
@@ -1157,36 +1138,36 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.15">
       <c r="E17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
@@ -1194,197 +1175,161 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B19" s="3"/>
+      <c r="B19" s="2"/>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B20" s="3"/>
+      <c r="B20" s="2"/>
       <c r="E20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B21" s="2"/>
+      <c r="E21" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B22" s="2"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B23" s="2"/>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B24" s="2"/>
+      <c r="E24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B25" s="2"/>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B27" s="2"/>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B28" s="2"/>
+      <c r="E28" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B29" s="2"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B30" s="2"/>
+      <c r="D30" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B21" s="3"/>
-      <c r="E21" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B22" s="3"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B23" s="3"/>
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B24" s="3"/>
-      <c r="E24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B25" s="3"/>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B27" s="3"/>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B28" s="3"/>
-      <c r="E28" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B29" s="3"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B30" s="3"/>
-      <c r="D30" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.15">
       <c r="E31" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="D32" s="4"/>
-      <c r="E32" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B35" s="3" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.15">
       <c r="D36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.15">
       <c r="E37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="F38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B40" s="2"/>
+      <c r="D40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="D44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="E41" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C45" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="D46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="F42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="F43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="F44" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="E45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="E46" t="s">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C49" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D51" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C52" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B55" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C56" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>